<commit_message>
Update Product Dimension.xlsx with latest product data
</commit_message>
<xml_diff>
--- a/backend/data/Product Dimension.xlsx
+++ b/backend/data/Product Dimension.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zackwu204/CursorAI/Sunique/02-shipping/development-website/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EC6B7A-473D-614C-A86E-892A3381883F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908A4731-5292-9040-A4A0-264168EDF5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assembled" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
     <t>SW-REP1.596</t>
   </si>
   <si>
-    <t>SW-VSD60</t>
+    <t>SW-VSD60S</t>
   </si>
 </sst>
 </file>
@@ -5197,7 +5197,7 @@
   <dimension ref="A1:F210"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>